<commit_message>
Minor updates to Excel workbooks
</commit_message>
<xml_diff>
--- a/decision_matrix.xlsx
+++ b/decision_matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewtait/Documents/projects/LearningTree/decision_analysis/load/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC4E189B-0358-1D41-A841-B2D63A08DBD9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89A49DE1-686A-AC40-B912-F7D7F7EAE142}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="35100" yWindow="5480" windowWidth="28040" windowHeight="17440" xr2:uid="{92A19090-7FE1-AD4C-9A8E-E793F88687E5}"/>
   </bookViews>
@@ -32,13 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
-  <si>
-    <t>Alternative</t>
-  </si>
-  <si>
-    <t>comform</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>styling</t>
   </si>
@@ -85,22 +79,25 @@
     <t>Ferrari Roma</t>
   </si>
   <si>
-    <t>Rank</t>
-  </si>
-  <si>
-    <t>Rating</t>
-  </si>
-  <si>
-    <t>Scores</t>
-  </si>
-  <si>
-    <t>Legend</t>
-  </si>
-  <si>
     <t>Input</t>
   </si>
   <si>
     <t>Result</t>
+  </si>
+  <si>
+    <t>comfort</t>
+  </si>
+  <si>
+    <t>scores</t>
+  </si>
+  <si>
+    <t>rating</t>
+  </si>
+  <si>
+    <t>rank</t>
+  </si>
+  <si>
+    <t>legend</t>
   </si>
 </sst>
 </file>
@@ -278,16 +275,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>57.5</c:v>
+                  <c:v>57.608897126969417</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>41.7</c:v>
+                  <c:v>41.65883247406947</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>69.3</c:v>
+                  <c:v>69.214231407435349</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>37.9</c:v>
+                  <c:v>37.725799559361356</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1378,126 +1375,126 @@
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1">
       <c r="B1" s="6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C1" s="6"/>
       <c r="D1" s="6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E1" s="6"/>
       <c r="F1" s="6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G1" s="6"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B2" s="7">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="7">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="E2" s="7"/>
       <c r="F2" s="7">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="G2" s="7"/>
       <c r="K2" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B3" s="5">
         <f>B2/SUM($B2:$G2)</f>
-        <v>0.2</v>
+        <v>0.19879518072289157</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5">
         <f t="shared" ref="D3" si="0">D2/SUM($B2:$G2)</f>
-        <v>0.2</v>
+        <v>0.19879518072289157</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="5">
         <f t="shared" ref="F3" si="1">F2/SUM($B2:$G2)</f>
-        <v>0.6</v>
+        <v>0.60240963855421692</v>
       </c>
       <c r="G3" s="5"/>
       <c r="K3" s="3" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:11" s="1" customFormat="1">
       <c r="B4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="K4" s="4" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B5" s="3">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="C5" s="3">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="D5" s="3">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="E5" s="3">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="F5" s="3">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="G5" s="3">
-        <v>50</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B6">
         <f>B5/SUM($B5:$C5)</f>
-        <v>0.6</v>
+        <v>0.59880239520958078</v>
       </c>
       <c r="C6">
         <f>C5/SUM($B5:$C5)</f>
-        <v>0.4</v>
+        <v>0.40119760479041916</v>
       </c>
       <c r="D6">
         <f>D5/SUM($D5:$E5)</f>
-        <v>0.3</v>
+        <v>0.30069930069930068</v>
       </c>
       <c r="E6">
         <f>E5/SUM($D5:$E5)</f>
-        <v>0.7</v>
+        <v>0.69930069930069927</v>
       </c>
       <c r="F6">
         <f>F5/SUM($F5:$G5)</f>
@@ -1510,40 +1507,37 @@
     </row>
     <row r="7" spans="1:11" s="1" customFormat="1">
       <c r="A7" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B7" s="1">
         <f>B6*$B3</f>
-        <v>0.12</v>
+        <v>0.11903903037298895</v>
       </c>
       <c r="C7" s="1">
         <f>C6*$B3</f>
-        <v>8.0000000000000016E-2</v>
+        <v>7.9756150349902605E-2</v>
       </c>
       <c r="D7" s="1">
         <f>D6*$D3</f>
-        <v>0.06</v>
+        <v>5.977757182576459E-2</v>
       </c>
       <c r="E7" s="1">
         <f>E6*$D3</f>
-        <v>0.13999999999999999</v>
+        <v>0.13901760889712697</v>
       </c>
       <c r="F7" s="1">
         <f>F6*$F3</f>
-        <v>0.3</v>
+        <v>0.30120481927710846</v>
       </c>
       <c r="G7" s="1">
         <f>G6*$F3</f>
-        <v>0.3</v>
+        <v>0.30120481927710846</v>
       </c>
     </row>
     <row r="8" spans="1:11" s="1" customFormat="1"/>
     <row r="9" spans="1:11" s="1" customFormat="1">
-      <c r="A9" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="B9" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
@@ -1551,15 +1545,15 @@
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
       <c r="H9" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:11">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B10" s="3">
         <v>30</v>
@@ -1581,7 +1575,7 @@
       </c>
       <c r="H10" s="2">
         <f>SUMPRODUCT(B$7:G$7, B10:G10)</f>
-        <v>57.5</v>
+        <v>57.608897126969417</v>
       </c>
       <c r="I10" s="2">
         <f>RANK(H10, H$10:H$13)</f>
@@ -1590,7 +1584,7 @@
     </row>
     <row r="11" spans="1:11">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B11" s="3">
         <v>100</v>
@@ -1612,7 +1606,7 @@
       </c>
       <c r="H11" s="2">
         <f t="shared" ref="H11:H13" si="2">SUMPRODUCT(B$7:G$7, B11:G11)</f>
-        <v>41.7</v>
+        <v>41.65883247406947</v>
       </c>
       <c r="I11" s="2">
         <f t="shared" ref="I11:I13" si="3">RANK(H11, H$10:H$13)</f>
@@ -1621,7 +1615,7 @@
     </row>
     <row r="12" spans="1:11">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B12" s="3">
         <v>100</v>
@@ -1643,7 +1637,7 @@
       </c>
       <c r="H12" s="2">
         <f t="shared" si="2"/>
-        <v>69.3</v>
+        <v>69.214231407435349</v>
       </c>
       <c r="I12" s="2">
         <f t="shared" si="3"/>
@@ -1652,7 +1646,7 @@
     </row>
     <row r="13" spans="1:11">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B13" s="3">
         <v>80</v>
@@ -1674,7 +1668,7 @@
       </c>
       <c r="H13" s="2">
         <f t="shared" si="2"/>
-        <v>37.9</v>
+        <v>37.725799559361356</v>
       </c>
       <c r="I13" s="2">
         <f t="shared" si="3"/>

</xml_diff>